<commit_message>
analog clock update and bugs fix
</commit_message>
<xml_diff>
--- a/circle_points.xlsx
+++ b/circle_points.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16470" windowHeight="6765"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16470" windowHeight="6770"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -146,11 +146,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="729119744"/>
-        <c:axId val="729128368"/>
+        <c:axId val="460433512"/>
+        <c:axId val="460431160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="729119744"/>
+        <c:axId val="460433512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -206,12 +206,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="729128368"/>
+        <c:crossAx val="460431160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="729128368"/>
+        <c:axId val="460431160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -268,7 +268,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="729119744"/>
+        <c:crossAx val="460433512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -390,187 +390,187 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
                 <c:pt idx="0">
-                  <c:v>95</c:v>
+                  <c:v>50.661644283866558</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>93</c:v>
+                  <c:v>43.239248141205159</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90</c:v>
+                  <c:v>37.55030101616039</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>84</c:v>
+                  <c:v>34.047981175235762</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>77</c:v>
+                  <c:v>33.011281409076801</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>69</c:v>
+                  <c:v>34.522784626714994</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>61</c:v>
+                  <c:v>38.46208534837919</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>53</c:v>
+                  <c:v>44.51538113698561</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>46</c:v>
+                  <c:v>52.200469920372761</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41</c:v>
+                  <c:v>60.905161931923047</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>36</c:v>
+                  <c:v>69.936046396402688</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>35</c:v>
+                  <c:v>78.5737282347839</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>36</c:v>
+                  <c:v>86.130134663810566</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>39</c:v>
+                  <c:v>92.003326679439752</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>45</c:v>
+                  <c:v>95.725449172811707</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>52</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>60</c:v>
+                  <c:v>95.725449172811707</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>68</c:v>
+                  <c:v>92.003326679439752</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>76</c:v>
+                  <c:v>86.130134663810566</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>84</c:v>
+                  <c:v>78.5737282347839</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>89</c:v>
+                  <c:v>69.936046396402688</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>93</c:v>
+                  <c:v>60.905161931923047</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>95</c:v>
+                  <c:v>52.200469920372761</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>94</c:v>
+                  <c:v>44.51538113698561</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>91</c:v>
+                  <c:v>38.46208534837919</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>86</c:v>
+                  <c:v>34.522784626714994</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>79</c:v>
+                  <c:v>33.011281409076801</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>71</c:v>
+                  <c:v>34.047981175235762</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>63</c:v>
+                  <c:v>37.55030101616039</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>54</c:v>
+                  <c:v>43.239248141205159</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>47</c:v>
+                  <c:v>50.661644283866558</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>41</c:v>
+                  <c:v>59.226225622685313</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>37</c:v>
+                  <c:v>68.250742518291887</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>35</c:v>
+                  <c:v>77.016307128544383</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>36</c:v>
+                  <c:v>84.824659601894723</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>38</c:v>
+                  <c:v>91.053791056849974</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>43</c:v>
+                  <c:v>95.20749245287405</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>50</c:v>
+                  <c:v>96.954882318079711</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>58</c:v>
+                  <c:v>96.156764577584582</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>66</c:v>
+                  <c:v>92.87671683303499</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>75</c:v>
+                  <c:v>87.376025807307997</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>82</c:v>
+                  <c:v>80.092873393962833</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>88</c:v>
+                  <c:v>71.60743133880996</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>93</c:v>
+                  <c:v>62.595645091252699</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>95</c:v>
+                  <c:v>53.77538837730782</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>94</c:v>
+                  <c:v>45.849277790148541</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>92</c:v>
+                  <c:v>39.448702755102964</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>87</c:v>
+                  <c:v>35.083529410008474</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>81</c:v>
+                  <c:v>33.101484960978219</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>73</c:v>
+                  <c:v>33.660457932514419</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>64</c:v>
+                  <c:v>36.715920858164104</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>56</c:v>
+                  <c:v>42.024477312969168</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>48</c:v>
+                  <c:v>49.163250733139122</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>42</c:v>
+                  <c:v>57.563570520687279</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>38</c:v>
+                  <c:v>66.556272017247011</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>35</c:v>
+                  <c:v>75.425001777124734</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>35</c:v>
+                  <c:v>83.463281872097866</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>38</c:v>
+                  <c:v>90.030787518152678</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>42</c:v>
+                  <c:v>94.604354980680256</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>49</c:v>
+                  <c:v>96.819656497645241</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>56</c:v>
+                  <c:v>96.500222420240164</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -582,187 +582,187 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="61"/>
                 <c:pt idx="0">
+                  <c:v>59.607893235217851</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>54.462090242345354</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47.447310591601124</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39.122347608385162</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.150363071233063</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.246060124729066</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.118750436748279</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.4158508376426617</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6713104666997189</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.73692331017970503</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.61701197097157845</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.0214924157880354</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.9684081033063663</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.829666623986082</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>22.058704057634372</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>53</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>58</c:v>
-                </c:pt>
                 <c:pt idx="16">
-                  <c:v>60</c:v>
+                  <c:v>39.941295942365628</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>61</c:v>
+                  <c:v>48.170333376013915</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>59</c:v>
+                  <c:v>55.031591896693634</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>54</c:v>
+                  <c:v>59.978507584211968</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>48</c:v>
+                  <c:v>62.617011970971575</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41</c:v>
+                  <c:v>62.736923310179705</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>33</c:v>
+                  <c:v>60.328689533300278</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>24</c:v>
+                  <c:v>55.584149162357335</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>16</c:v>
+                  <c:v>48.881249563251721</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9</c:v>
+                  <c:v>40.75393987527093</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4</c:v>
+                  <c:v>31.849636928766937</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2</c:v>
+                  <c:v>22.877652391614838</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1</c:v>
+                  <c:v>14.552689408398873</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3</c:v>
+                  <c:v>7.5379097576546492</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7</c:v>
+                  <c:v>2.3921067647821488</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>13</c:v>
+                  <c:v>-0.47480785389903701</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>20</c:v>
+                  <c:v>-0.83445732346900314</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>29</c:v>
+                  <c:v>1.3418078266308804</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>37</c:v>
+                  <c:v>5.8806275621980646</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>45</c:v>
+                  <c:v>12.420442105205943</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>52</c:v>
+                  <c:v>20.440293578438975</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>57</c:v>
+                  <c:v>29.301325211326137</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>60</c:v>
+                  <c:v>38.297672304027557</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>61</c:v>
+                  <c:v>46.712691004751022</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>59</c:v>
+                  <c:v>53.876045748133265</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>55</c:v>
+                  <c:v>59.217107802072995</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>50</c:v>
+                  <c:v>62.310411225388151</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>42</c:v>
+                  <c:v>62.909545240770555</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>34</c:v>
+                  <c:v>60.966783176038824</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>26</c:v>
+                  <c:v>56.636884343482578</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>18</c:v>
+                  <c:v>50.264766001769061</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>11</c:v>
+                  <c:v>42.358027444859083</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>5</c:v>
+                  <c:v>33.546514933257072</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2</c:v>
+                  <c:v>24.532148501990683</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1</c:v>
+                  <c:v>16.033007413031712</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2</c:v>
+                  <c:v>8.7261283729628332</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>6</c:v>
+                  <c:v>3.1935731770768214</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>12</c:v>
+                  <c:v>-0.12393799953997942</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>19</c:v>
+                  <c:v>-0.96213411848986397</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>27</c:v>
+                  <c:v>0.74575504252426228</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>35</c:v>
+                  <c:v>4.8636800120701267</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>44</c:v>
+                  <c:v>11.063609247883104</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>51</c:v>
+                  <c:v>18.851659941462302</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>56</c:v>
+                  <c:v>27.607440439452361</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>60</c:v>
+                  <c:v>36.633470287078765</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -777,11 +777,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="729127976"/>
-        <c:axId val="729122488"/>
+        <c:axId val="460434296"/>
+        <c:axId val="460437432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="729127976"/>
+        <c:axId val="460434296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -838,12 +838,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="729122488"/>
+        <c:crossAx val="460437432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="729122488"/>
+        <c:axId val="460437432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -900,7 +900,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="729127976"/>
+        <c:crossAx val="460434296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2095,16 +2095,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>157161</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>130175</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>49211</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>358775</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>73024</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2392,12 +2392,12 @@
   <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S32" sqref="S32"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -2414,17 +2414,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="B2">
         <f>H$2+J$2*COS(A2)</f>
-        <v>95</v>
+        <v>50.661644283866558</v>
       </c>
       <c r="C2">
         <f>I$2+J$2*SIN(A2)</f>
-        <v>31</v>
+        <v>59.607893235217851</v>
       </c>
       <c r="H2">
         <v>65</v>
@@ -2433,667 +2433,787 @@
         <v>31</v>
       </c>
       <c r="J2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>84</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B62" si="0">H$2+J$2*COS(A3)</f>
+        <v>43.239248141205159</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C62" si="1">I$2+J$2*SIN(A3)</f>
+        <v>54.462090242345354</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>78</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>37.55030101616039</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>47.447310591601124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>72</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>34.047981175235762</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>39.122347608385162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>66</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>33.011281409076801</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>30.150363071233063</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>60</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>34.522784626714994</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>21.246060124729066</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>54</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>38.46208534837919</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>13.118750436748279</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>48</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>44.51538113698561</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>6.4158508376426617</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>42</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>52.200469920372761</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>1.6713104666997189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>36</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>60.905161931923047</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>-0.73692331017970503</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>69.936046396402688</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>-0.61701197097157845</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>78.5737282347839</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>2.0214924157880354</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>86.130134663810566</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>6.9684081033063663</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>92.003326679439752</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>13.829666623986082</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>93</v>
-      </c>
-      <c r="C3">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>90</v>
-      </c>
-      <c r="C4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>18</v>
-      </c>
-      <c r="B5">
-        <v>84</v>
-      </c>
-      <c r="C5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>24</v>
-      </c>
-      <c r="B6">
-        <v>77</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>30</v>
-      </c>
-      <c r="B7">
-        <v>69</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>36</v>
-      </c>
-      <c r="B8">
-        <v>61</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>42</v>
-      </c>
-      <c r="B9">
-        <v>53</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>48</v>
-      </c>
-      <c r="B10">
-        <v>46</v>
-      </c>
-      <c r="C10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>54</v>
-      </c>
-      <c r="B11">
-        <v>41</v>
-      </c>
-      <c r="C11">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>60</v>
-      </c>
-      <c r="B12">
-        <v>36</v>
-      </c>
-      <c r="C12">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>66</v>
-      </c>
-      <c r="B13">
-        <v>35</v>
-      </c>
-      <c r="C13">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>72</v>
-      </c>
-      <c r="B14">
-        <v>36</v>
-      </c>
-      <c r="C14">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>78</v>
-      </c>
-      <c r="B15">
-        <v>39</v>
-      </c>
-      <c r="C15">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>84</v>
-      </c>
       <c r="B16">
-        <v>45</v>
+        <f t="shared" si="0"/>
+        <v>95.725449172811707</v>
       </c>
       <c r="C16">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>22.058704057634372</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="B17">
-        <v>52</v>
+        <f t="shared" si="0"/>
+        <v>97</v>
       </c>
       <c r="C17">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>96</v>
+        <v>-6</v>
       </c>
       <c r="B18">
-        <v>60</v>
+        <f t="shared" si="0"/>
+        <v>95.725449172811707</v>
       </c>
       <c r="C18">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>39.941295942365628</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>102</v>
+        <v>-12</v>
       </c>
       <c r="B19">
-        <v>68</v>
+        <f t="shared" si="0"/>
+        <v>92.003326679439752</v>
       </c>
       <c r="C19">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>48.170333376013915</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>108</v>
+        <v>-18</v>
       </c>
       <c r="B20">
-        <v>76</v>
+        <f t="shared" si="0"/>
+        <v>86.130134663810566</v>
       </c>
       <c r="C20">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>55.031591896693634</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>114</v>
+        <v>-24</v>
       </c>
       <c r="B21">
-        <v>84</v>
+        <f t="shared" si="0"/>
+        <v>78.5737282347839</v>
       </c>
       <c r="C21">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>59.978507584211968</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>120</v>
+        <v>-30</v>
       </c>
       <c r="B22">
-        <v>89</v>
+        <f t="shared" si="0"/>
+        <v>69.936046396402688</v>
       </c>
       <c r="C22">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>62.617011970971575</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>126</v>
+        <v>-36</v>
       </c>
       <c r="B23">
-        <v>93</v>
+        <f t="shared" si="0"/>
+        <v>60.905161931923047</v>
       </c>
       <c r="C23">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>62.736923310179705</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>132</v>
+        <v>-42</v>
       </c>
       <c r="B24">
-        <v>95</v>
+        <f t="shared" si="0"/>
+        <v>52.200469920372761</v>
       </c>
       <c r="C24">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>60.328689533300278</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>138</v>
+        <v>-48</v>
       </c>
       <c r="B25">
-        <v>94</v>
+        <f t="shared" si="0"/>
+        <v>44.51538113698561</v>
       </c>
       <c r="C25">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>55.584149162357335</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>144</v>
+        <v>-54</v>
       </c>
       <c r="B26">
-        <v>91</v>
+        <f t="shared" si="0"/>
+        <v>38.46208534837919</v>
       </c>
       <c r="C26">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>48.881249563251721</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>150</v>
+        <v>-60</v>
       </c>
       <c r="B27">
-        <v>86</v>
+        <f t="shared" si="0"/>
+        <v>34.522784626714994</v>
       </c>
       <c r="C27">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>40.75393987527093</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>156</v>
+        <v>-66</v>
       </c>
       <c r="B28">
-        <v>79</v>
+        <f t="shared" si="0"/>
+        <v>33.011281409076801</v>
       </c>
       <c r="C28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>31.849636928766937</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>162</v>
+        <v>-72</v>
       </c>
       <c r="B29">
-        <v>71</v>
+        <f t="shared" si="0"/>
+        <v>34.047981175235762</v>
       </c>
       <c r="C29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>22.877652391614838</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>168</v>
+        <v>-78</v>
       </c>
       <c r="B30">
-        <v>63</v>
+        <f t="shared" si="0"/>
+        <v>37.55030101616039</v>
       </c>
       <c r="C30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>14.552689408398873</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>174</v>
+        <v>-84</v>
       </c>
       <c r="B31">
-        <v>54</v>
+        <f t="shared" si="0"/>
+        <v>43.239248141205159</v>
       </c>
       <c r="C31">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>7.5379097576546492</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>180</v>
+        <v>-90</v>
       </c>
       <c r="B32">
-        <v>47</v>
+        <f t="shared" si="0"/>
+        <v>50.661644283866558</v>
       </c>
       <c r="C32">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>2.3921067647821488</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>186</v>
+        <v>-96</v>
       </c>
       <c r="B33">
-        <v>41</v>
+        <f t="shared" si="0"/>
+        <v>59.226225622685313</v>
       </c>
       <c r="C33">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-0.47480785389903701</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>192</v>
+        <v>-102</v>
       </c>
       <c r="B34">
-        <v>37</v>
+        <f t="shared" si="0"/>
+        <v>68.250742518291887</v>
       </c>
       <c r="C34">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-0.83445732346900314</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>198</v>
+        <v>-108</v>
       </c>
       <c r="B35">
-        <v>35</v>
+        <f t="shared" si="0"/>
+        <v>77.016307128544383</v>
       </c>
       <c r="C35">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1.3418078266308804</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
-        <v>204</v>
+        <v>-114</v>
       </c>
       <c r="B36">
-        <v>36</v>
+        <f t="shared" si="0"/>
+        <v>84.824659601894723</v>
       </c>
       <c r="C36">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>5.8806275621980646</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>210</v>
+        <v>-120</v>
       </c>
       <c r="B37">
-        <v>38</v>
+        <f t="shared" si="0"/>
+        <v>91.053791056849974</v>
       </c>
       <c r="C37">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>12.420442105205943</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
-        <v>216</v>
+        <v>-126</v>
       </c>
       <c r="B38">
-        <v>43</v>
+        <f t="shared" si="0"/>
+        <v>95.20749245287405</v>
       </c>
       <c r="C38">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>20.440293578438975</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39">
-        <v>222</v>
+        <v>-132</v>
       </c>
       <c r="B39">
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>96.954882318079711</v>
       </c>
       <c r="C39">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>29.301325211326137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
-        <v>228</v>
+        <v>-138</v>
       </c>
       <c r="B40">
-        <v>58</v>
+        <f t="shared" si="0"/>
+        <v>96.156764577584582</v>
       </c>
       <c r="C40">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>38.297672304027557</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41">
-        <v>234</v>
+        <v>-144</v>
       </c>
       <c r="B41">
-        <v>66</v>
+        <f t="shared" si="0"/>
+        <v>92.87671683303499</v>
       </c>
       <c r="C41">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>46.712691004751022</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42">
-        <v>240</v>
+        <v>-150</v>
       </c>
       <c r="B42">
-        <v>75</v>
+        <f t="shared" si="0"/>
+        <v>87.376025807307997</v>
       </c>
       <c r="C42">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>53.876045748133265</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43">
-        <v>246</v>
+        <v>-156</v>
       </c>
       <c r="B43">
-        <v>82</v>
+        <f t="shared" si="0"/>
+        <v>80.092873393962833</v>
       </c>
       <c r="C43">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>59.217107802072995</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44">
-        <v>252</v>
+        <v>-162</v>
       </c>
       <c r="B44">
-        <v>88</v>
+        <f t="shared" si="0"/>
+        <v>71.60743133880996</v>
       </c>
       <c r="C44">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>62.310411225388151</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45">
-        <v>258</v>
+        <v>-168</v>
       </c>
       <c r="B45">
-        <v>93</v>
+        <f t="shared" si="0"/>
+        <v>62.595645091252699</v>
       </c>
       <c r="C45">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>62.909545240770555</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46">
-        <v>264</v>
+        <v>-174</v>
       </c>
       <c r="B46">
-        <v>95</v>
+        <f t="shared" si="0"/>
+        <v>53.77538837730782</v>
       </c>
       <c r="C46">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>60.966783176038824</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47">
-        <v>270</v>
+        <v>-180</v>
       </c>
       <c r="B47">
-        <v>94</v>
+        <f t="shared" si="0"/>
+        <v>45.849277790148541</v>
       </c>
       <c r="C47">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>56.636884343482578</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48">
-        <v>276</v>
+        <v>-186</v>
       </c>
       <c r="B48">
-        <v>92</v>
+        <f t="shared" si="0"/>
+        <v>39.448702755102964</v>
       </c>
       <c r="C48">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>50.264766001769061</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49">
-        <v>282</v>
+        <v>-192</v>
       </c>
       <c r="B49">
-        <v>87</v>
+        <f t="shared" si="0"/>
+        <v>35.083529410008474</v>
       </c>
       <c r="C49">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>42.358027444859083</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50">
-        <v>288</v>
+        <v>-198</v>
       </c>
       <c r="B50">
-        <v>81</v>
+        <f t="shared" si="0"/>
+        <v>33.101484960978219</v>
       </c>
       <c r="C50">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>33.546514933257072</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51">
-        <v>294</v>
+        <v>-204</v>
       </c>
       <c r="B51">
-        <v>73</v>
+        <f t="shared" si="0"/>
+        <v>33.660457932514419</v>
       </c>
       <c r="C51">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>24.532148501990683</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52">
-        <v>300</v>
+        <v>-210</v>
       </c>
       <c r="B52">
-        <v>64</v>
+        <f t="shared" si="0"/>
+        <v>36.715920858164104</v>
       </c>
       <c r="C52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>16.033007413031712</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53">
-        <v>306</v>
+        <v>-216</v>
       </c>
       <c r="B53">
-        <v>56</v>
+        <f t="shared" si="0"/>
+        <v>42.024477312969168</v>
       </c>
       <c r="C53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>8.7261283729628332</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54">
-        <v>312</v>
+        <v>-222</v>
       </c>
       <c r="B54">
-        <v>48</v>
+        <f t="shared" si="0"/>
+        <v>49.163250733139122</v>
       </c>
       <c r="C54">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>3.1935731770768214</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55">
-        <v>318</v>
+        <v>-228</v>
       </c>
       <c r="B55">
-        <v>42</v>
+        <f t="shared" si="0"/>
+        <v>57.563570520687279</v>
       </c>
       <c r="C55">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-0.12393799953997942</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56">
-        <v>324</v>
+        <v>-234</v>
       </c>
       <c r="B56">
-        <v>38</v>
+        <f t="shared" si="0"/>
+        <v>66.556272017247011</v>
       </c>
       <c r="C56">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-0.96213411848986397</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57">
-        <v>330</v>
+        <v>-240</v>
       </c>
       <c r="B57">
-        <v>35</v>
+        <f t="shared" si="0"/>
+        <v>75.425001777124734</v>
       </c>
       <c r="C57">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0.74575504252426228</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58">
-        <v>336</v>
+        <v>-246</v>
       </c>
       <c r="B58">
-        <v>35</v>
+        <f t="shared" si="0"/>
+        <v>83.463281872097866</v>
       </c>
       <c r="C58">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>4.8636800120701267</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59">
-        <v>342</v>
+        <v>-252</v>
       </c>
       <c r="B59">
-        <v>38</v>
+        <f t="shared" si="0"/>
+        <v>90.030787518152678</v>
       </c>
       <c r="C59">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>11.063609247883104</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60">
-        <v>348</v>
+        <v>-258</v>
       </c>
       <c r="B60">
-        <v>42</v>
+        <f t="shared" si="0"/>
+        <v>94.604354980680256</v>
       </c>
       <c r="C60">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>18.851659941462302</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61">
-        <v>354</v>
+        <v>-264</v>
       </c>
       <c r="B61">
-        <v>49</v>
+        <f t="shared" si="0"/>
+        <v>96.819656497645241</v>
       </c>
       <c r="C61">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>27.607440439452361</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62">
-        <v>360</v>
+        <v>-270</v>
       </c>
       <c r="B62">
-        <v>56</v>
+        <f t="shared" si="0"/>
+        <v>96.500222420240164</v>
       </c>
       <c r="C62">
-        <v>60</v>
+        <f t="shared" si="1"/>
+        <v>36.633470287078765</v>
       </c>
     </row>
   </sheetData>

</xml_diff>